<commit_message>
Domingo 20 junio - Luly
</commit_message>
<xml_diff>
--- a/DATA/AdminSubcuentaDeVivienda.xlsx
+++ b/DATA/AdminSubcuentaDeVivienda.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lulyelizondo/Documents/tesis/DATA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C473CD9-C817-BC4F-B2C0-3A62D2FFCE6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4246C27-3B2D-7140-AB2B-77E2AB9AD9C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -493,7 +493,7 @@
   <dimension ref="A1:D101"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>